<commit_message>
feat(excel): update download links for vehicle companies and engines Excel files; enhance button layout for better readability
</commit_message>
<xml_diff>
--- a/rabbit_service_d_app/assets/vehicle_companies_list.xlsx
+++ b/rabbit_service_d_app/assets/vehicle_companies_list.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\F-Drive-Data\MylexCompanyProjects\rabbit_services_project\rabbit_service_d_app\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E982C0E-1198-4C23-BC10-B0CC3B8EB062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Truck Manufacturers" sheetId="1" r:id="rId1"/>
-    <sheet name="Trailer Manufacturers" sheetId="2" r:id="rId2"/>
+    <sheet name="Truck company Name and Engine" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Company Name</t>
   </si>
@@ -23,9 +28,6 @@
     <t>Vehicle Type</t>
   </si>
   <si>
-    <t>FREIGHTLINER</t>
-  </si>
-  <si>
     <t>HINO MOTORS</t>
   </si>
   <si>
@@ -53,32 +55,38 @@
     <t>Truck</t>
   </si>
   <si>
-    <t>DRY VAN</t>
-  </si>
-  <si>
-    <t>GREAT DANE</t>
-  </si>
-  <si>
-    <t>HYUNDAI</t>
-  </si>
-  <si>
-    <t>UTILITY</t>
-  </si>
-  <si>
-    <t>VANGUARD</t>
-  </si>
-  <si>
-    <t>WABASH</t>
-  </si>
-  <si>
-    <t>Trailer</t>
+    <t>Engine Name</t>
+  </si>
+  <si>
+    <t>CUMMINS</t>
+  </si>
+  <si>
+    <t>DETROIT</t>
+  </si>
+  <si>
+    <t>MAXFORCE</t>
+  </si>
+  <si>
+    <t>NAVISTAR</t>
+  </si>
+  <si>
+    <t>CATERPILLER</t>
+  </si>
+  <si>
+    <t>PACCAR</t>
+  </si>
+  <si>
+    <t>MERCEDES BENZ</t>
+  </si>
+  <si>
+    <t>FREIGHTlINEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,7 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -141,13 +153,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +205,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -219,6 +239,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -253,9 +274,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,160 +450,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>